<commit_message>
CIs do NB no Model Results
</commit_message>
<xml_diff>
--- a/atividade6-Naive Bayes/PCA/scores_balanced-PCA_NB.xlsx
+++ b/atividade6-Naive Bayes/PCA/scores_balanced-PCA_NB.xlsx
@@ -1260,13 +1260,13 @@
         <v>3</v>
       </c>
       <c r="D44">
-        <v>0.4</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E44">
         <v>0.8</v>
       </c>
       <c r="F44">
-        <v>0.9186046511627907</v>
+        <v>0.9302325581395349</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1920,13 +1920,13 @@
         <v>6</v>
       </c>
       <c r="D77">
-        <v>0.8</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E77">
         <v>0.6666666666666666</v>
       </c>
       <c r="F77">
-        <v>0.9651162790697675</v>
+        <v>0.9534883720930233</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -2320,13 +2320,13 @@
         <v>6</v>
       </c>
       <c r="D97">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="E97">
         <v>0.6666666666666666</v>
       </c>
       <c r="F97">
-        <v>0.9767441860465116</v>
+        <v>0.9651162790697675</v>
       </c>
     </row>
     <row r="98" spans="1:6">

</xml_diff>